<commit_message>
build order creator error handling
</commit_message>
<xml_diff>
--- a/documentation/error_handling_plan.xlsx
+++ b/documentation/error_handling_plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\RTSanalytics\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59ABB0A2-C040-4C3B-AB4B-9B22FB0C5FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20EB555F-22BA-4FDD-A528-0284205759D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13935" yWindow="0" windowWidth="14970" windowHeight="15585" xr2:uid="{3DB1A640-9907-4B89-8561-12BCDA8399FC}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{3DB1A640-9907-4B89-8561-12BCDA8399FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="102">
   <si>
     <t>File</t>
   </si>
@@ -270,9 +270,6 @@
   </si>
   <si>
     <t>Weight should be a value between 0-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">raise error </t>
   </si>
   <si>
     <t>Command __ weight of __ is not between 0-1</t>
@@ -368,7 +365,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -387,6 +384,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -400,7 +403,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -415,6 +418,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -753,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D084F35-09EF-4F5B-B0E7-BE4C51EA3C9B}">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,7 +826,7 @@
         <v>58</v>
       </c>
       <c r="C2" s="1">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>65</v>
@@ -840,7 +846,7 @@
       <c r="I2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="3"/>
+      <c r="J2" s="6"/>
       <c r="K2" s="5"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -851,7 +857,7 @@
         <v>58</v>
       </c>
       <c r="C3" s="1">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>62</v>
@@ -871,7 +877,7 @@
       <c r="I3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="3"/>
+      <c r="J3" s="6"/>
       <c r="K3" s="5"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -882,7 +888,7 @@
         <v>58</v>
       </c>
       <c r="C4" s="1">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>66</v>
@@ -902,7 +908,7 @@
       <c r="I4" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="J4" s="3"/>
+      <c r="J4" s="6"/>
       <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -913,7 +919,7 @@
         <v>58</v>
       </c>
       <c r="C5" s="1">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>70</v>
@@ -933,7 +939,7 @@
       <c r="I5" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="J5" s="3"/>
+      <c r="J5" s="6"/>
       <c r="K5" s="5"/>
     </row>
     <row r="6" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -947,7 +953,7 @@
         <v>55</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>11</v>
@@ -964,7 +970,7 @@
       <c r="I6" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="J6" s="3"/>
+      <c r="J6" s="6"/>
       <c r="K6" s="5"/>
       <c r="L6" s="2"/>
     </row>
@@ -985,18 +991,18 @@
         <v>11</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="J7" s="3"/>
+      <c r="J7" s="6"/>
       <c r="K7" s="5"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1010,13 +1016,13 @@
         <v>99</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>12</v>
@@ -1076,13 +1082,13 @@
         <v>149</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>12</v>
@@ -1109,13 +1115,13 @@
         <v>47</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>12</v>
@@ -1139,13 +1145,13 @@
         <v>48</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>12</v>
@@ -1163,19 +1169,19 @@
         <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C13" s="1">
         <v>101</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>12</v>
@@ -1193,19 +1199,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C14" s="1">
         <v>102</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>12</v>
@@ -1220,100 +1226,100 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="C15" s="1">
         <v>35</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="J15" s="3"/>
     </row>
     <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C16" s="1">
         <v>36</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F16" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="J16" s="3"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C17" s="1">
         <v>58</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F17" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" s="1" t="s">
         <v>92</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="J17" s="3"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="C18" s="1">
         <v>24</v>
@@ -1343,31 +1349,31 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C19" s="1">
         <v>49</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>36</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="1" t="s">
@@ -1427,7 +1433,7 @@
         <v>36</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J21" s="3"/>
       <c r="K21" s="1" t="s">
@@ -1457,7 +1463,7 @@
         <v>36</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J22" s="3"/>
       <c r="K22" s="1" t="s">
@@ -1487,7 +1493,7 @@
         <v>36</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J23" s="3"/>
       <c r="K23" s="1" t="s">

</xml_diff>